<commit_message>
added html reporting, fixed a bug in duplicated ID
</commit_message>
<xml_diff>
--- a/test_resource/Testcases.xlsx
+++ b/test_resource/Testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" checkCompatibility="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PythonRepo\text-de-duplication\test_resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PythonRepo\delete\TextSimilarityProcessor\test_resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Test Case(ID / Brief Description)</t>
   </si>
@@ -54,125 +54,88 @@
     <t>a</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>d2</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>a3</t>
-  </si>
-  <si>
-    <t>d4</t>
-  </si>
-  <si>
-    <t>qqq</t>
-  </si>
-  <si>
-    <t>qwerty</t>
-  </si>
-  <si>
-    <t>mnbghd</t>
-  </si>
-  <si>
-    <t>cccc12</t>
-  </si>
-  <si>
-    <t>qwwqwq33</t>
-  </si>
-  <si>
     <t>TC_099</t>
   </si>
   <si>
-    <t>abcdefg</t>
-  </si>
-  <si>
-    <t>a11</t>
-  </si>
-  <si>
     <t>TC_100</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
-    <t>yy</t>
-  </si>
-  <si>
-    <t>er</t>
-  </si>
-  <si>
-    <t>gf</t>
-  </si>
-  <si>
-    <t>vv</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>sss</t>
-  </si>
-  <si>
-    <t>rg</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
-    <t>dfjgh</t>
-  </si>
-  <si>
-    <t>Pyt</t>
-  </si>
-  <si>
-    <t>hon</t>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>sample test</t>
+  </si>
+  <si>
+    <t>try the</t>
+  </si>
+  <si>
+    <t>similarity</t>
+  </si>
+  <si>
+    <t>of text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is </t>
+  </si>
+  <si>
+    <t>generate</t>
+  </si>
+  <si>
+    <t>the similarity</t>
+  </si>
+  <si>
+    <t>this is a sample test to generate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on </t>
+  </si>
+  <si>
+    <t>similarity processor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is a simple dummy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">this should not get </t>
+  </si>
+  <si>
+    <t>called</t>
+  </si>
+  <si>
+    <t>these are random</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>this test case can call to other</t>
+  </si>
+  <si>
+    <t>so get it and</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -221,6 +184,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,38 +499,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="134" customWidth="1"/>
-    <col min="5" max="28" width="255" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="255" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -580,23 +547,19 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -618,20 +581,16 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="C3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -654,46 +613,39 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -716,20 +668,14 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -752,21 +698,15 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -788,15 +728,11 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="1"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -820,18 +756,16 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
+      <c r="B11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -856,16 +790,16 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
+      <c r="B12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -890,127 +824,120 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="20" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>101</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>101</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>3</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="10" t="s">
         <v>17</v>
       </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1034,30 +961,24 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>101</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>3</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="B27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1065,6 +986,7 @@
     <mergeCell ref="A17:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>